<commit_message>
Septimo comit del proyecto, modificacion del codigo para verificar que todos los productos tengan Titulo, Abstract, Pimer autor, Año de publicación, Tipo de producto, Journal
</commit_message>
<xml_diff>
--- a/Variables bases de datos.xlsx
+++ b/Variables bases de datos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad\Analisis Algoritmos 2024-2\Proyecto_Final_Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3836379-C512-454B-B8FB-9AE4D1DC96AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B3B6D1-F69A-4CF9-9927-2F690513A0B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5868" yWindow="72" windowWidth="17280" windowHeight="9420" xr2:uid="{525E8FEC-E55C-49E6-A982-D6705CBF2B69}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{525E8FEC-E55C-49E6-A982-D6705CBF2B69}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="36">
   <si>
     <t>ID</t>
   </si>
@@ -662,16 +662,16 @@
   <dimension ref="A3:S131"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1"/>
-    <col min="4" max="4" width="26.109375" customWidth="1"/>
-    <col min="5" max="5" width="21.33203125" customWidth="1"/>
+    <col min="3" max="3" width="40.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="113.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="185.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:19" s="3" customFormat="1" ht="115.2" x14ac:dyDescent="0.55000000000000004">
@@ -753,7 +753,9 @@
       <c r="A6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="10"/>
+      <c r="B6" s="10" t="s">
+        <v>1</v>
+      </c>
       <c r="C6" s="10" t="s">
         <v>1</v>
       </c>

</xml_diff>